<commit_message>
more records for ram
</commit_message>
<xml_diff>
--- a/R/deploytimes/monitoringresults.xlsx
+++ b/R/deploytimes/monitoringresults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ansible" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="109">
   <si>
     <t>cpu</t>
   </si>
@@ -357,12 +357,15 @@
   <si>
     <t>ansible</t>
   </si>
+  <si>
+    <t>mariadb=stopped</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -399,6 +402,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +475,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -493,6 +503,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -502,7 +515,48 @@
     <cellStyle name="Procent" xfId="5" builtinId="5"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1102,11 +1156,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1050674400"/>
-        <c:axId val="964286592"/>
+        <c:axId val="-946668288"/>
+        <c:axId val="-946665728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1050674400"/>
+        <c:axId val="-946668288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1202,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="964286592"/>
+        <c:crossAx val="-946665728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1156,7 +1210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="964286592"/>
+        <c:axId val="-946665728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1260,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050674400"/>
+        <c:crossAx val="-946668288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1429,11 +1483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="986836112"/>
-        <c:axId val="986838432"/>
+        <c:axId val="-946538464"/>
+        <c:axId val="-946535712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="986836112"/>
+        <c:axId val="-946538464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1529,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="986838432"/>
+        <c:crossAx val="-946535712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1483,7 +1537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="986838432"/>
+        <c:axId val="-946535712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1588,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="986836112"/>
+        <c:crossAx val="-946538464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1711,11 +1765,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="983870272"/>
-        <c:axId val="982332256"/>
+        <c:axId val="-1016543552"/>
+        <c:axId val="-1016540864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="983870272"/>
+        <c:axId val="-1016543552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1811,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="982332256"/>
+        <c:crossAx val="-1016540864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1765,7 +1819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="982332256"/>
+        <c:axId val="-1016540864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,6 +1839,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1815,7 +1870,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="983870272"/>
+        <c:crossAx val="-1016543552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1904,7 +1959,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1996,11 +2050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1048816064"/>
-        <c:axId val="1048817840"/>
+        <c:axId val="-1016507232"/>
+        <c:axId val="-1016504432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1048816064"/>
+        <c:axId val="-1016507232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,7 +2096,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048817840"/>
+        <c:crossAx val="-1016504432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2050,7 +2104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1048817840"/>
+        <c:axId val="-1016504432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2155,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048816064"/>
+        <c:crossAx val="-1016507232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2190,7 +2244,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2285,11 +2338,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1050231904"/>
-        <c:axId val="1050233680"/>
+        <c:axId val="-947334032"/>
+        <c:axId val="-947331280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1050231904"/>
+        <c:axId val="-947334032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2331,7 +2384,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050233680"/>
+        <c:crossAx val="-947331280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2339,7 +2392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1050233680"/>
+        <c:axId val="-947331280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,7 +2442,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050231904"/>
+        <c:crossAx val="-947334032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2478,7 +2531,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2567,11 +2619,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="960241616"/>
-        <c:axId val="960243936"/>
+        <c:axId val="-946517856"/>
+        <c:axId val="-946515104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="960241616"/>
+        <c:axId val="-946517856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2613,7 +2665,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="960243936"/>
+        <c:crossAx val="-946515104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2621,7 +2673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="960243936"/>
+        <c:axId val="-946515104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2671,7 +2723,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="960241616"/>
+        <c:crossAx val="-946517856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2854,11 +2906,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1050085296"/>
-        <c:axId val="960368880"/>
+        <c:axId val="-947424928"/>
+        <c:axId val="-947320176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1050085296"/>
+        <c:axId val="-947424928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2900,7 +2952,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="960368880"/>
+        <c:crossAx val="-947320176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2908,7 +2960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="960368880"/>
+        <c:axId val="-947320176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2959,7 +3011,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050085296"/>
+        <c:crossAx val="-947424928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3153,11 +3205,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="960459312"/>
-        <c:axId val="1050059936"/>
+        <c:axId val="-946487152"/>
+        <c:axId val="-946484400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="960459312"/>
+        <c:axId val="-946487152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +3251,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050059936"/>
+        <c:crossAx val="-946484400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3207,7 +3259,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1050059936"/>
+        <c:axId val="-946484400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3258,7 +3310,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="960459312"/>
+        <c:crossAx val="-946487152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3491,11 +3543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="888460288"/>
-        <c:axId val="960051168"/>
+        <c:axId val="-947290800"/>
+        <c:axId val="-947288048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="888460288"/>
+        <c:axId val="-947290800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3537,7 +3589,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="960051168"/>
+        <c:crossAx val="-947288048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3545,7 +3597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="960051168"/>
+        <c:axId val="-947288048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3596,7 +3648,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="888460288"/>
+        <c:crossAx val="-947290800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3860,11 +3912,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1049822016"/>
-        <c:axId val="960226352"/>
+        <c:axId val="-947270480"/>
+        <c:axId val="-947267728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1049822016"/>
+        <c:axId val="-947270480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3906,7 +3958,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="960226352"/>
+        <c:crossAx val="-947267728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3914,7 +3966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="960226352"/>
+        <c:axId val="-947267728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3964,7 +4016,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049822016"/>
+        <c:crossAx val="-947270480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4234,11 +4286,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="984092736"/>
-        <c:axId val="961319968"/>
+        <c:axId val="-946457680"/>
+        <c:axId val="-946454928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="984092736"/>
+        <c:axId val="-946457680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4280,7 +4332,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="961319968"/>
+        <c:crossAx val="-946454928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4288,7 +4340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="961319968"/>
+        <c:axId val="-946454928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4393,7 +4445,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="984092736"/>
+        <c:crossAx val="-946457680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5034,11 +5086,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1050842704"/>
-        <c:axId val="1050869312"/>
+        <c:axId val="-946596768"/>
+        <c:axId val="-946593776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1050842704"/>
+        <c:axId val="-946596768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5080,7 +5132,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050869312"/>
+        <c:crossAx val="-946593776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5088,7 +5140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1050869312"/>
+        <c:axId val="-946593776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5168,7 +5220,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050842704"/>
+        <c:crossAx val="-946596768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5855,11 +5907,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1048802160"/>
-        <c:axId val="984527392"/>
+        <c:axId val="-1016575184"/>
+        <c:axId val="-1016573040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1048802160"/>
+        <c:axId val="-1016575184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5901,7 +5953,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="984527392"/>
+        <c:crossAx val="-1016573040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5909,7 +5961,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="984527392"/>
+        <c:axId val="-1016573040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5959,6 +6011,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5989,7 +6042,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048802160"/>
+        <c:crossAx val="-1016575184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6296,8 +6349,8 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1049658288"/>
-        <c:axId val="1049913520"/>
+        <c:axId val="-947466480"/>
+        <c:axId val="-947464160"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6655,11 +6708,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="960431584"/>
-        <c:axId val="960450576"/>
+        <c:axId val="-947459520"/>
+        <c:axId val="-947461840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1049658288"/>
+        <c:axId val="-947466480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6696,7 +6749,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049913520"/>
+        <c:crossAx val="-947464160"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6704,7 +6757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1049913520"/>
+        <c:axId val="-947464160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6755,12 +6808,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049658288"/>
+        <c:crossAx val="-947466480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="960450576"/>
+        <c:axId val="-947461840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6770,12 +6823,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="960431584"/>
+        <c:crossAx val="-947459520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="960431584"/>
+        <c:axId val="-947459520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6784,7 +6837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="960450576"/>
+        <c:crossAx val="-947461840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6915,7 +6968,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7017,11 +7069,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1048673424"/>
-        <c:axId val="1049037168"/>
+        <c:axId val="-1015117792"/>
+        <c:axId val="-1015146240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1048673424"/>
+        <c:axId val="-1015117792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7063,7 +7115,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1049037168"/>
+        <c:crossAx val="-1015146240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7071,7 +7123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1049037168"/>
+        <c:axId val="-1015146240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7122,7 +7174,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1048673424"/>
+        <c:crossAx val="-1015117792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7211,7 +7263,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7303,11 +7354,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1050216800"/>
-        <c:axId val="1050219120"/>
+        <c:axId val="-1015075936"/>
+        <c:axId val="-947727040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1050216800"/>
+        <c:axId val="-1015075936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7349,7 +7400,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050219120"/>
+        <c:crossAx val="-947727040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7357,7 +7408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1050219120"/>
+        <c:axId val="-947727040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7377,6 +7428,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7407,7 +7459,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050216800"/>
+        <c:crossAx val="-1015075936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7496,7 +7548,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7591,11 +7642,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="959116208"/>
-        <c:axId val="986754112"/>
+        <c:axId val="-947375168"/>
+        <c:axId val="-947372416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="959116208"/>
+        <c:axId val="-947375168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7637,7 +7688,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="986754112"/>
+        <c:crossAx val="-947372416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7645,7 +7696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="986754112"/>
+        <c:axId val="-947372416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7695,7 +7746,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="959116208"/>
+        <c:crossAx val="-947375168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7784,7 +7835,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7876,11 +7926,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="958060112"/>
-        <c:axId val="957741232"/>
+        <c:axId val="-947364720"/>
+        <c:axId val="-947361968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="958060112"/>
+        <c:axId val="-947364720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7922,7 +7972,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="957741232"/>
+        <c:crossAx val="-947361968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7930,7 +7980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="957741232"/>
+        <c:axId val="-947361968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7980,7 +8030,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="958060112"/>
+        <c:crossAx val="-947364720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8163,11 +8213,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="984613984"/>
-        <c:axId val="958222352"/>
+        <c:axId val="-947350224"/>
+        <c:axId val="-947347472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="984613984"/>
+        <c:axId val="-947350224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8209,7 +8259,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="958222352"/>
+        <c:crossAx val="-947347472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8217,7 +8267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="958222352"/>
+        <c:axId val="-947347472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8267,7 +8317,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="984613984"/>
+        <c:crossAx val="-947350224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19685,10 +19735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M102"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L103" sqref="L103"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21786,7 +21836,692 @@
         <v>981</v>
       </c>
     </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A105" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108" s="28">
+        <v>28.45</v>
+      </c>
+      <c r="B108" s="29">
+        <v>46.62</v>
+      </c>
+      <c r="C108" s="29">
+        <v>38.17</v>
+      </c>
+      <c r="D108" s="29">
+        <v>50.78</v>
+      </c>
+      <c r="E108" s="29">
+        <v>49.33</v>
+      </c>
+      <c r="F108" s="29">
+        <v>40.54</v>
+      </c>
+      <c r="G108" s="29">
+        <v>31.5</v>
+      </c>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
+      <c r="L108" s="16">
+        <f>AVERAGE(B108:K108)</f>
+        <v>42.823333333333323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" s="28">
+        <v>28.48</v>
+      </c>
+      <c r="B109" s="29">
+        <v>33.229999999999997</v>
+      </c>
+      <c r="C109" s="29">
+        <v>40.31</v>
+      </c>
+      <c r="D109" s="29">
+        <v>41.26</v>
+      </c>
+      <c r="E109" s="29">
+        <v>50.89</v>
+      </c>
+      <c r="F109" s="29">
+        <v>49.7</v>
+      </c>
+      <c r="G109" s="29">
+        <v>40.630000000000003</v>
+      </c>
+      <c r="H109" s="29">
+        <v>31.49</v>
+      </c>
+      <c r="I109" s="29"/>
+      <c r="L109" s="16">
+        <f t="shared" ref="L109:L129" si="0">AVERAGE(B109:K109)</f>
+        <v>41.072857142857139</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A110" s="28">
+        <v>29.17</v>
+      </c>
+      <c r="B110" s="29">
+        <v>46.64</v>
+      </c>
+      <c r="C110" s="29">
+        <v>44.1</v>
+      </c>
+      <c r="D110" s="29">
+        <v>50.83</v>
+      </c>
+      <c r="E110" s="29">
+        <v>52.12</v>
+      </c>
+      <c r="F110" s="29">
+        <v>32.17</v>
+      </c>
+      <c r="G110" s="29"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="29"/>
+      <c r="L110" s="16">
+        <f t="shared" si="0"/>
+        <v>45.172000000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A111" s="28">
+        <v>28.41</v>
+      </c>
+      <c r="B111" s="29">
+        <v>31.28</v>
+      </c>
+      <c r="C111" s="29">
+        <v>46.75</v>
+      </c>
+      <c r="D111" s="29">
+        <v>44.14</v>
+      </c>
+      <c r="E111" s="29">
+        <v>50.86</v>
+      </c>
+      <c r="F111" s="29">
+        <v>49.93</v>
+      </c>
+      <c r="G111" s="29">
+        <v>32.9</v>
+      </c>
+      <c r="H111" s="29">
+        <v>31.6</v>
+      </c>
+      <c r="I111" s="29"/>
+      <c r="L111" s="16">
+        <f t="shared" si="0"/>
+        <v>41.065714285714293</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A112" s="28">
+        <v>28.44</v>
+      </c>
+      <c r="B112" s="29">
+        <v>41.05</v>
+      </c>
+      <c r="C112" s="29">
+        <v>39.67</v>
+      </c>
+      <c r="D112" s="29">
+        <v>50.74</v>
+      </c>
+      <c r="E112" s="29">
+        <v>50.82</v>
+      </c>
+      <c r="F112" s="29">
+        <v>48.81</v>
+      </c>
+      <c r="G112" s="29">
+        <v>33.43</v>
+      </c>
+      <c r="H112" s="29">
+        <v>31.51</v>
+      </c>
+      <c r="I112" s="29"/>
+      <c r="L112" s="16">
+        <f t="shared" si="0"/>
+        <v>42.29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A113" s="28">
+        <v>28.69</v>
+      </c>
+      <c r="B113" s="29">
+        <v>46.71</v>
+      </c>
+      <c r="C113" s="29">
+        <v>41.26</v>
+      </c>
+      <c r="D113" s="29">
+        <v>50.8</v>
+      </c>
+      <c r="E113" s="29">
+        <v>48.44</v>
+      </c>
+      <c r="F113" s="29">
+        <v>31.66</v>
+      </c>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="L113" s="16">
+        <f t="shared" si="0"/>
+        <v>43.773999999999994</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A114" s="28">
+        <v>28.42</v>
+      </c>
+      <c r="B114" s="29">
+        <v>31.46</v>
+      </c>
+      <c r="C114" s="29">
+        <v>38.67</v>
+      </c>
+      <c r="D114" s="29">
+        <v>49.11</v>
+      </c>
+      <c r="E114" s="29">
+        <v>50.86</v>
+      </c>
+      <c r="F114" s="29">
+        <v>52.09</v>
+      </c>
+      <c r="G114" s="29">
+        <v>41.17</v>
+      </c>
+      <c r="H114" s="29">
+        <v>31.43</v>
+      </c>
+      <c r="I114" s="29"/>
+      <c r="L114" s="16">
+        <f t="shared" si="0"/>
+        <v>42.112857142857145</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A115" s="28">
+        <v>28.43</v>
+      </c>
+      <c r="B115" s="29">
+        <v>34.86</v>
+      </c>
+      <c r="C115" s="29">
+        <v>39.869999999999997</v>
+      </c>
+      <c r="D115" s="29">
+        <v>50.74</v>
+      </c>
+      <c r="E115" s="29">
+        <v>50.85</v>
+      </c>
+      <c r="F115" s="29">
+        <v>48.82</v>
+      </c>
+      <c r="G115" s="29">
+        <v>31.49</v>
+      </c>
+      <c r="H115" s="29"/>
+      <c r="I115" s="29"/>
+      <c r="L115" s="16">
+        <f t="shared" si="0"/>
+        <v>42.771666666666668</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A116" s="28">
+        <v>28.42</v>
+      </c>
+      <c r="B116" s="29">
+        <v>38.58</v>
+      </c>
+      <c r="C116" s="29">
+        <v>37.19</v>
+      </c>
+      <c r="D116" s="29">
+        <v>34.72</v>
+      </c>
+      <c r="E116" s="29">
+        <v>50.79</v>
+      </c>
+      <c r="F116" s="29">
+        <v>53.09</v>
+      </c>
+      <c r="G116" s="29">
+        <v>49.02</v>
+      </c>
+      <c r="H116" s="29">
+        <v>31.82</v>
+      </c>
+      <c r="I116" s="29"/>
+      <c r="L116" s="16">
+        <f t="shared" si="0"/>
+        <v>42.17285714285714</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A117" s="28">
+        <v>28.41</v>
+      </c>
+      <c r="B117" s="29">
+        <v>33.97</v>
+      </c>
+      <c r="C117" s="29">
+        <v>38.630000000000003</v>
+      </c>
+      <c r="D117" s="29">
+        <v>49.6</v>
+      </c>
+      <c r="E117" s="29">
+        <v>50.86</v>
+      </c>
+      <c r="F117" s="29">
+        <v>55.29</v>
+      </c>
+      <c r="G117" s="29">
+        <v>40.42</v>
+      </c>
+      <c r="H117" s="29">
+        <v>31.72</v>
+      </c>
+      <c r="I117" s="29"/>
+      <c r="L117" s="16">
+        <f t="shared" si="0"/>
+        <v>42.927142857142861</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A118" s="28">
+        <v>28.14</v>
+      </c>
+      <c r="B118" s="29">
+        <v>42.31</v>
+      </c>
+      <c r="C118" s="29">
+        <v>36.57</v>
+      </c>
+      <c r="D118" s="29">
+        <v>41.56</v>
+      </c>
+      <c r="E118" s="29">
+        <v>50.33</v>
+      </c>
+      <c r="F118" s="29">
+        <v>54.77</v>
+      </c>
+      <c r="G118" s="29">
+        <v>41.76</v>
+      </c>
+      <c r="H118" s="29">
+        <v>31.21</v>
+      </c>
+      <c r="I118" s="29"/>
+      <c r="L118" s="16">
+        <f t="shared" si="0"/>
+        <v>42.644285714285715</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A119" s="28">
+        <v>27.77</v>
+      </c>
+      <c r="B119" s="29">
+        <v>30.66</v>
+      </c>
+      <c r="C119" s="29">
+        <v>45.93</v>
+      </c>
+      <c r="D119" s="29">
+        <v>40.549999999999997</v>
+      </c>
+      <c r="E119" s="29">
+        <v>50.22</v>
+      </c>
+      <c r="F119" s="29">
+        <v>50.24</v>
+      </c>
+      <c r="G119" s="29">
+        <v>50.27</v>
+      </c>
+      <c r="H119" s="29">
+        <v>48.3</v>
+      </c>
+      <c r="I119" s="29">
+        <v>31.49</v>
+      </c>
+      <c r="L119" s="16">
+        <f t="shared" si="0"/>
+        <v>43.457500000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A120" s="28">
+        <v>27.8</v>
+      </c>
+      <c r="B120" s="29">
+        <v>40.44</v>
+      </c>
+      <c r="C120" s="29">
+        <v>37.76</v>
+      </c>
+      <c r="D120" s="29">
+        <v>50.21</v>
+      </c>
+      <c r="E120" s="29">
+        <v>50.25</v>
+      </c>
+      <c r="F120" s="29">
+        <v>51.82</v>
+      </c>
+      <c r="G120" s="29">
+        <v>46.83</v>
+      </c>
+      <c r="H120" s="29">
+        <v>31.22</v>
+      </c>
+      <c r="I120" s="29"/>
+      <c r="L120" s="16">
+        <f t="shared" si="0"/>
+        <v>44.075714285714284</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A121" s="28">
+        <v>27.84</v>
+      </c>
+      <c r="B121" s="29">
+        <v>40.54</v>
+      </c>
+      <c r="C121" s="29">
+        <v>46.02</v>
+      </c>
+      <c r="D121" s="29">
+        <v>35.36</v>
+      </c>
+      <c r="E121" s="29">
+        <v>50.27</v>
+      </c>
+      <c r="F121" s="29">
+        <v>50.29</v>
+      </c>
+      <c r="G121" s="29">
+        <v>54.06</v>
+      </c>
+      <c r="H121" s="29">
+        <v>41.29</v>
+      </c>
+      <c r="I121" s="29">
+        <v>31.21</v>
+      </c>
+      <c r="L121" s="16">
+        <f t="shared" si="0"/>
+        <v>43.629999999999995</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A122" s="28">
+        <v>27.84</v>
+      </c>
+      <c r="B122" s="29">
+        <v>29.36</v>
+      </c>
+      <c r="C122" s="29">
+        <v>46.03</v>
+      </c>
+      <c r="D122" s="29">
+        <v>43.23</v>
+      </c>
+      <c r="E122" s="29">
+        <v>50.35</v>
+      </c>
+      <c r="F122" s="29">
+        <v>52.6</v>
+      </c>
+      <c r="G122" s="29">
+        <v>48.49</v>
+      </c>
+      <c r="H122" s="29">
+        <v>31.52</v>
+      </c>
+      <c r="I122" s="29"/>
+      <c r="L122" s="16">
+        <f t="shared" si="0"/>
+        <v>43.082857142857144</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A123" s="28">
+        <v>27.82</v>
+      </c>
+      <c r="B123" s="29">
+        <v>33.44</v>
+      </c>
+      <c r="C123" s="29">
+        <v>47.45</v>
+      </c>
+      <c r="D123" s="29">
+        <v>38.56</v>
+      </c>
+      <c r="E123" s="29">
+        <v>50.27</v>
+      </c>
+      <c r="F123" s="29">
+        <v>50.3</v>
+      </c>
+      <c r="G123" s="29">
+        <v>48.29</v>
+      </c>
+      <c r="H123" s="29">
+        <v>31.38</v>
+      </c>
+      <c r="I123" s="29"/>
+      <c r="L123" s="16">
+        <f t="shared" si="0"/>
+        <v>42.812857142857141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A124" s="28">
+        <v>27.82</v>
+      </c>
+      <c r="B124" s="29">
+        <v>40.76</v>
+      </c>
+      <c r="C124" s="29">
+        <v>34.26</v>
+      </c>
+      <c r="D124" s="29">
+        <v>50.26</v>
+      </c>
+      <c r="E124" s="29">
+        <v>52.57</v>
+      </c>
+      <c r="F124" s="29">
+        <v>51.02</v>
+      </c>
+      <c r="G124" s="29">
+        <v>32.659999999999997</v>
+      </c>
+      <c r="H124" s="29"/>
+      <c r="I124" s="29"/>
+      <c r="L124" s="16">
+        <f t="shared" si="0"/>
+        <v>43.588333333333331</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A125" s="28">
+        <v>28.15</v>
+      </c>
+      <c r="B125" s="29">
+        <v>41.08</v>
+      </c>
+      <c r="C125" s="29">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="D125" s="29">
+        <v>50.27</v>
+      </c>
+      <c r="E125" s="29">
+        <v>52.62</v>
+      </c>
+      <c r="F125" s="29">
+        <v>41.39</v>
+      </c>
+      <c r="G125" s="29">
+        <v>31.26</v>
+      </c>
+      <c r="H125" s="29"/>
+      <c r="I125" s="29"/>
+      <c r="L125" s="16">
+        <f t="shared" si="0"/>
+        <v>41.82</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A126" s="28">
+        <v>27.84</v>
+      </c>
+      <c r="B126" s="29">
+        <v>30.76</v>
+      </c>
+      <c r="C126" s="29">
+        <v>46.02</v>
+      </c>
+      <c r="D126" s="29">
+        <v>43.56</v>
+      </c>
+      <c r="E126" s="29">
+        <v>50.32</v>
+      </c>
+      <c r="F126" s="29">
+        <v>51.91</v>
+      </c>
+      <c r="G126" s="29">
+        <v>40.24</v>
+      </c>
+      <c r="H126" s="29">
+        <v>31.21</v>
+      </c>
+      <c r="I126" s="29"/>
+      <c r="L126" s="16">
+        <f t="shared" si="0"/>
+        <v>42.002857142857138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A127" s="28">
+        <v>27.83</v>
+      </c>
+      <c r="B127" s="29">
+        <v>37.97</v>
+      </c>
+      <c r="C127" s="29">
+        <v>40.130000000000003</v>
+      </c>
+      <c r="D127" s="29">
+        <v>45.08</v>
+      </c>
+      <c r="E127" s="29">
+        <v>50.32</v>
+      </c>
+      <c r="F127" s="29">
+        <v>50.28</v>
+      </c>
+      <c r="G127" s="29">
+        <v>48.38</v>
+      </c>
+      <c r="H127" s="29">
+        <v>31.46</v>
+      </c>
+      <c r="I127" s="29"/>
+      <c r="L127" s="16">
+        <f t="shared" si="0"/>
+        <v>43.374285714285712</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A128" s="28">
+        <v>28.09</v>
+      </c>
+      <c r="B128" s="29">
+        <v>42.83</v>
+      </c>
+      <c r="C128" s="29">
+        <v>35.520000000000003</v>
+      </c>
+      <c r="D128" s="29">
+        <v>50.24</v>
+      </c>
+      <c r="E128" s="29">
+        <v>50.32</v>
+      </c>
+      <c r="F128" s="29">
+        <v>48.39</v>
+      </c>
+      <c r="G128" s="29">
+        <v>32.78</v>
+      </c>
+      <c r="H128" s="29">
+        <v>32.22</v>
+      </c>
+      <c r="I128" s="29"/>
+      <c r="L128" s="16">
+        <f t="shared" si="0"/>
+        <v>41.757142857142867</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A129" s="28">
+        <v>27.9</v>
+      </c>
+      <c r="B129" s="29">
+        <v>40.79</v>
+      </c>
+      <c r="C129" s="29">
+        <v>40.65</v>
+      </c>
+      <c r="D129" s="29">
+        <v>50.3</v>
+      </c>
+      <c r="E129" s="29">
+        <v>50.35</v>
+      </c>
+      <c r="F129" s="29">
+        <v>50.89</v>
+      </c>
+      <c r="G129" s="29">
+        <v>41.84</v>
+      </c>
+      <c r="H129" s="29">
+        <v>31.27</v>
+      </c>
+      <c r="I129" s="29"/>
+      <c r="L129" s="16">
+        <f t="shared" si="0"/>
+        <v>43.727142857142859</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A108:I129">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>34</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -21796,8 +22531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView topLeftCell="A94" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24815,7 +25550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="Y23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="86" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="86" workbookViewId="0">
       <selection activeCell="N56" sqref="N56:O56"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more memory results for puppet and ansible
</commit_message>
<xml_diff>
--- a/R/deploytimes/monitoringresults.xlsx
+++ b/R/deploytimes/monitoringresults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ansible" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="111">
   <si>
     <t>cpu</t>
   </si>
@@ -360,6 +360,12 @@
   <si>
     <t>mariadb=stopped</t>
   </si>
+  <si>
+    <t xml:space="preserve">memorye </t>
+  </si>
+  <si>
+    <t>mariadb not running</t>
+  </si>
 </sst>
 </file>
 
@@ -515,7 +521,87 @@
     <cellStyle name="Procent" xfId="5" builtinId="5"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -606,6 +692,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1274,6 +1361,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18883,15 +18971,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>371336</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:colOff>371335</xdr:colOff>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>96629</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>138044</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>82825</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>193260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19737,8 +19825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="J123" sqref="J123"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22518,7 +22606,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A108:I129">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>34</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22529,10 +22617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U104"/>
+  <dimension ref="A1:U147"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75:J75"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
+      <selection activeCell="K122" sqref="K122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25189,7 +25277,770 @@
         <v>1820</v>
       </c>
     </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>38.020000000000003</v>
+      </c>
+      <c r="B126">
+        <v>48.85</v>
+      </c>
+      <c r="C126">
+        <v>64.39</v>
+      </c>
+      <c r="D126">
+        <v>58.46</v>
+      </c>
+      <c r="E126">
+        <v>67.23</v>
+      </c>
+      <c r="F126">
+        <v>68.150000000000006</v>
+      </c>
+      <c r="G126">
+        <v>63.54</v>
+      </c>
+      <c r="H126">
+        <v>57.98</v>
+      </c>
+      <c r="I126">
+        <v>39.22</v>
+      </c>
+      <c r="T126" s="23">
+        <f>AVERAGE(A126:S126)</f>
+        <v>56.204444444444448</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>37.42</v>
+      </c>
+      <c r="B127">
+        <v>46.06</v>
+      </c>
+      <c r="C127">
+        <v>57.93</v>
+      </c>
+      <c r="D127">
+        <v>57.77</v>
+      </c>
+      <c r="E127">
+        <v>65.97</v>
+      </c>
+      <c r="F127">
+        <v>68.31</v>
+      </c>
+      <c r="G127">
+        <v>63.2</v>
+      </c>
+      <c r="H127">
+        <v>53.36</v>
+      </c>
+      <c r="I127">
+        <v>38.659999999999997</v>
+      </c>
+      <c r="T127" s="23">
+        <f t="shared" ref="T127:T147" si="0">AVERAGE(A127:S127)</f>
+        <v>54.297777777777775</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="B128">
+        <v>42.26</v>
+      </c>
+      <c r="C128">
+        <v>57.95</v>
+      </c>
+      <c r="D128">
+        <v>55.13</v>
+      </c>
+      <c r="E128">
+        <v>66</v>
+      </c>
+      <c r="F128">
+        <v>67.53</v>
+      </c>
+      <c r="G128">
+        <v>67.56</v>
+      </c>
+      <c r="H128">
+        <v>62.64</v>
+      </c>
+      <c r="I128">
+        <v>45.18</v>
+      </c>
+      <c r="J128">
+        <v>38.93</v>
+      </c>
+      <c r="T128" s="23">
+        <f t="shared" si="0"/>
+        <v>54.088000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>36.67</v>
+      </c>
+      <c r="B129">
+        <v>41.61</v>
+      </c>
+      <c r="C129">
+        <v>58.03</v>
+      </c>
+      <c r="D129">
+        <v>56.97</v>
+      </c>
+      <c r="E129">
+        <v>65.13</v>
+      </c>
+      <c r="F129">
+        <v>66.72</v>
+      </c>
+      <c r="G129">
+        <v>62.52</v>
+      </c>
+      <c r="H129">
+        <v>53.49</v>
+      </c>
+      <c r="I129">
+        <v>42.39</v>
+      </c>
+      <c r="T129" s="23">
+        <f t="shared" si="0"/>
+        <v>53.725555555555552</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>36.99</v>
+      </c>
+      <c r="B130">
+        <v>41.3</v>
+      </c>
+      <c r="C130">
+        <v>48.8</v>
+      </c>
+      <c r="D130">
+        <v>57.57</v>
+      </c>
+      <c r="E130">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="F130">
+        <v>67.319999999999993</v>
+      </c>
+      <c r="G130">
+        <v>63</v>
+      </c>
+      <c r="H130">
+        <v>51.31</v>
+      </c>
+      <c r="I130">
+        <v>41.55</v>
+      </c>
+      <c r="J130">
+        <v>38.71</v>
+      </c>
+      <c r="T130" s="23">
+        <f t="shared" si="0"/>
+        <v>51.155999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="B131">
+        <v>41.61</v>
+      </c>
+      <c r="C131">
+        <v>57.52</v>
+      </c>
+      <c r="D131">
+        <v>54.85</v>
+      </c>
+      <c r="E131">
+        <v>61.38</v>
+      </c>
+      <c r="F131">
+        <v>66.61</v>
+      </c>
+      <c r="G131">
+        <v>62.32</v>
+      </c>
+      <c r="H131">
+        <v>53.7</v>
+      </c>
+      <c r="I131">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="T131" s="23">
+        <f t="shared" si="0"/>
+        <v>52.681111111111107</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>38</v>
+      </c>
+      <c r="B132">
+        <v>48.7</v>
+      </c>
+      <c r="C132">
+        <v>61.46</v>
+      </c>
+      <c r="D132">
+        <v>60.96</v>
+      </c>
+      <c r="E132">
+        <v>66.709999999999994</v>
+      </c>
+      <c r="F132">
+        <v>62.36</v>
+      </c>
+      <c r="G132">
+        <v>54.25</v>
+      </c>
+      <c r="H132">
+        <v>42.47</v>
+      </c>
+      <c r="I132">
+        <v>39.19</v>
+      </c>
+      <c r="T132" s="23">
+        <f t="shared" si="0"/>
+        <v>52.677777777777777</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>36.69</v>
+      </c>
+      <c r="B133">
+        <v>41.75</v>
+      </c>
+      <c r="C133">
+        <v>57.98</v>
+      </c>
+      <c r="D133">
+        <v>51.38</v>
+      </c>
+      <c r="E133">
+        <v>66.52</v>
+      </c>
+      <c r="F133">
+        <v>68.44</v>
+      </c>
+      <c r="G133">
+        <v>62.63</v>
+      </c>
+      <c r="H133">
+        <v>47.55</v>
+      </c>
+      <c r="I133">
+        <v>38.74</v>
+      </c>
+      <c r="T133" s="23">
+        <f t="shared" si="0"/>
+        <v>52.408888888888889</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>37.33</v>
+      </c>
+      <c r="B134">
+        <v>45.9</v>
+      </c>
+      <c r="C134">
+        <v>64.3</v>
+      </c>
+      <c r="D134">
+        <v>57.66</v>
+      </c>
+      <c r="E134">
+        <v>67.31</v>
+      </c>
+      <c r="F134">
+        <v>67.22</v>
+      </c>
+      <c r="G134">
+        <v>53.91</v>
+      </c>
+      <c r="H134">
+        <v>39.159999999999997</v>
+      </c>
+      <c r="T134" s="23">
+        <f t="shared" si="0"/>
+        <v>54.098749999999995</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>37.03</v>
+      </c>
+      <c r="B135">
+        <v>41.58</v>
+      </c>
+      <c r="C135">
+        <v>48.73</v>
+      </c>
+      <c r="D135">
+        <v>57.59</v>
+      </c>
+      <c r="E135">
+        <v>57.75</v>
+      </c>
+      <c r="F135">
+        <v>67.14</v>
+      </c>
+      <c r="G135">
+        <v>67.95</v>
+      </c>
+      <c r="H135">
+        <v>62.56</v>
+      </c>
+      <c r="I135">
+        <v>55.44</v>
+      </c>
+      <c r="J135">
+        <v>38.83</v>
+      </c>
+      <c r="T135" s="23">
+        <f t="shared" si="0"/>
+        <v>53.46</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>37</v>
+      </c>
+      <c r="B136">
+        <v>42.37</v>
+      </c>
+      <c r="C136">
+        <v>59.58</v>
+      </c>
+      <c r="D136">
+        <v>55.64</v>
+      </c>
+      <c r="E136">
+        <v>58.48</v>
+      </c>
+      <c r="F136">
+        <v>67.23</v>
+      </c>
+      <c r="G136">
+        <v>67.08</v>
+      </c>
+      <c r="H136">
+        <v>62.18</v>
+      </c>
+      <c r="I136">
+        <v>53.87</v>
+      </c>
+      <c r="J136">
+        <v>38.65</v>
+      </c>
+      <c r="T136" s="23">
+        <f t="shared" si="0"/>
+        <v>54.207999999999991</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>37</v>
+      </c>
+      <c r="B137">
+        <v>41.61</v>
+      </c>
+      <c r="C137">
+        <v>57.97</v>
+      </c>
+      <c r="D137">
+        <v>54.09</v>
+      </c>
+      <c r="E137">
+        <v>66.489999999999995</v>
+      </c>
+      <c r="F137">
+        <v>68.040000000000006</v>
+      </c>
+      <c r="G137">
+        <v>66.36</v>
+      </c>
+      <c r="H137">
+        <v>51.82</v>
+      </c>
+      <c r="I137">
+        <v>39.090000000000003</v>
+      </c>
+      <c r="T137" s="23">
+        <f t="shared" si="0"/>
+        <v>53.607777777777784</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>37.03</v>
+      </c>
+      <c r="B138">
+        <v>48.05</v>
+      </c>
+      <c r="C138">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="D138">
+        <v>57.52</v>
+      </c>
+      <c r="E138">
+        <v>67.27</v>
+      </c>
+      <c r="F138">
+        <v>68.38</v>
+      </c>
+      <c r="G138">
+        <v>62.5</v>
+      </c>
+      <c r="H138">
+        <v>45.87</v>
+      </c>
+      <c r="I138">
+        <v>38.659999999999997</v>
+      </c>
+      <c r="T138" s="23">
+        <f t="shared" si="0"/>
+        <v>54.400000000000006</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>36.69</v>
+      </c>
+      <c r="B139">
+        <v>41.63</v>
+      </c>
+      <c r="C139">
+        <v>57.97</v>
+      </c>
+      <c r="D139">
+        <v>55.94</v>
+      </c>
+      <c r="E139">
+        <v>65.91</v>
+      </c>
+      <c r="F139">
+        <v>67.98</v>
+      </c>
+      <c r="G139">
+        <v>68.05</v>
+      </c>
+      <c r="H139">
+        <v>58.06</v>
+      </c>
+      <c r="I139">
+        <v>43.89</v>
+      </c>
+      <c r="J139">
+        <v>38.49</v>
+      </c>
+      <c r="T139" s="23">
+        <f t="shared" si="0"/>
+        <v>53.460999999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>37.69</v>
+      </c>
+      <c r="B140">
+        <v>48.63</v>
+      </c>
+      <c r="C140">
+        <v>63.75</v>
+      </c>
+      <c r="D140">
+        <v>58.6</v>
+      </c>
+      <c r="E140">
+        <v>65.06</v>
+      </c>
+      <c r="F140">
+        <v>66.849999999999994</v>
+      </c>
+      <c r="G140">
+        <v>62.89</v>
+      </c>
+      <c r="H140">
+        <v>47.65</v>
+      </c>
+      <c r="I140">
+        <v>38.99</v>
+      </c>
+      <c r="T140" s="23">
+        <f t="shared" si="0"/>
+        <v>54.456666666666671</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>37.31</v>
+      </c>
+      <c r="B141">
+        <v>45.07</v>
+      </c>
+      <c r="C141">
+        <v>61.34</v>
+      </c>
+      <c r="D141">
+        <v>56.72</v>
+      </c>
+      <c r="E141">
+        <v>67.33</v>
+      </c>
+      <c r="F141">
+        <v>68.22</v>
+      </c>
+      <c r="G141">
+        <v>57.82</v>
+      </c>
+      <c r="H141">
+        <v>46.82</v>
+      </c>
+      <c r="I141">
+        <v>41.8</v>
+      </c>
+      <c r="J141">
+        <v>38.76</v>
+      </c>
+      <c r="T141" s="23">
+        <f t="shared" si="0"/>
+        <v>52.119000000000007</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>36.99</v>
+      </c>
+      <c r="B142">
+        <v>42.2</v>
+      </c>
+      <c r="C142">
+        <v>57.28</v>
+      </c>
+      <c r="D142">
+        <v>55.5</v>
+      </c>
+      <c r="E142">
+        <v>65.739999999999995</v>
+      </c>
+      <c r="F142">
+        <v>67.319999999999993</v>
+      </c>
+      <c r="G142">
+        <v>49.68</v>
+      </c>
+      <c r="H142">
+        <v>42.23</v>
+      </c>
+      <c r="I142">
+        <v>39.369999999999997</v>
+      </c>
+      <c r="T142" s="23">
+        <f t="shared" si="0"/>
+        <v>50.701111111111111</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>36.69</v>
+      </c>
+      <c r="B143">
+        <v>41.3</v>
+      </c>
+      <c r="C143">
+        <v>48.8</v>
+      </c>
+      <c r="D143">
+        <v>64.3</v>
+      </c>
+      <c r="E143">
+        <v>57.73</v>
+      </c>
+      <c r="F143">
+        <v>64.5</v>
+      </c>
+      <c r="G143">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="H143">
+        <v>66.38</v>
+      </c>
+      <c r="I143">
+        <v>62.41</v>
+      </c>
+      <c r="J143">
+        <v>53.99</v>
+      </c>
+      <c r="K143">
+        <v>38.83</v>
+      </c>
+      <c r="T143" s="23">
+        <f t="shared" si="0"/>
+        <v>54.593636363636364</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>37.67</v>
+      </c>
+      <c r="B144">
+        <v>48.66</v>
+      </c>
+      <c r="C144">
+        <v>60.56</v>
+      </c>
+      <c r="D144">
+        <v>58.47</v>
+      </c>
+      <c r="E144">
+        <v>65.7</v>
+      </c>
+      <c r="F144">
+        <v>66.319999999999993</v>
+      </c>
+      <c r="G144">
+        <v>62.3</v>
+      </c>
+      <c r="H144">
+        <v>49.6</v>
+      </c>
+      <c r="I144">
+        <v>38.51</v>
+      </c>
+      <c r="T144" s="23">
+        <f t="shared" si="0"/>
+        <v>54.198888888888888</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>37.33</v>
+      </c>
+      <c r="B145">
+        <v>48.02</v>
+      </c>
+      <c r="C145">
+        <v>64.34</v>
+      </c>
+      <c r="D145">
+        <v>56.08</v>
+      </c>
+      <c r="E145">
+        <v>65.73</v>
+      </c>
+      <c r="F145">
+        <v>66.510000000000005</v>
+      </c>
+      <c r="G145">
+        <v>57.94</v>
+      </c>
+      <c r="H145">
+        <v>43.94</v>
+      </c>
+      <c r="I145">
+        <v>38.840000000000003</v>
+      </c>
+      <c r="T145" s="23">
+        <f t="shared" si="0"/>
+        <v>53.192222222222227</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>36.89</v>
+      </c>
+      <c r="B146">
+        <v>44.85</v>
+      </c>
+      <c r="C146">
+        <v>57.86</v>
+      </c>
+      <c r="D146">
+        <v>48.88</v>
+      </c>
+      <c r="E146">
+        <v>66.55</v>
+      </c>
+      <c r="F146">
+        <v>68.41</v>
+      </c>
+      <c r="G146">
+        <v>57.49</v>
+      </c>
+      <c r="H146">
+        <v>44.51</v>
+      </c>
+      <c r="I146">
+        <v>38.18</v>
+      </c>
+      <c r="T146" s="23">
+        <f t="shared" si="0"/>
+        <v>51.513333333333343</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>37.770000000000003</v>
+      </c>
+      <c r="B147">
+        <v>48.71</v>
+      </c>
+      <c r="C147">
+        <v>64.349999999999994</v>
+      </c>
+      <c r="D147">
+        <v>57.59</v>
+      </c>
+      <c r="E147">
+        <v>66.52</v>
+      </c>
+      <c r="F147">
+        <v>68.03</v>
+      </c>
+      <c r="G147">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="H147">
+        <v>57.86</v>
+      </c>
+      <c r="I147">
+        <v>52.6</v>
+      </c>
+      <c r="J147">
+        <v>38.71</v>
+      </c>
+      <c r="T147" s="23">
+        <f t="shared" si="0"/>
+        <v>56.004000000000005</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A126:J147 K143">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+      <formula>40</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feedback Lambrecht (typo's) verwerkt
</commit_message>
<xml_diff>
--- a/R/deploytimes/monitoringresults.xlsx
+++ b/R/deploytimes/monitoringresults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Ansible" sheetId="1" r:id="rId1"/>
@@ -718,6 +718,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1387,6 +1388,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20959,7 +20961,7 @@
   <dimension ref="A1:N233"/>
   <sheetViews>
     <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="L108" sqref="L108:L129"/>
+      <selection activeCell="A108" sqref="A108:I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23965,8 +23967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U189"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScale="63" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
-      <selection activeCell="T126" sqref="T126:T147"/>
+    <sheetView topLeftCell="A101" zoomScale="63" zoomScaleNormal="92" zoomScalePageLayoutView="92" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:K147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27624,8 +27626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
solved design issue + Puppet network dataset cleanup (laden van pagina veroorzaakte incorrecte resultaten)
</commit_message>
<xml_diff>
--- a/R/deploytimes/monitoringresults.xlsx
+++ b/R/deploytimes/monitoringresults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Ansible" sheetId="1" r:id="rId1"/>
@@ -718,7 +718,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1269,11 +1268,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448253408"/>
-        <c:axId val="448487744"/>
+        <c:axId val="1537403936"/>
+        <c:axId val="1537406496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448253408"/>
+        <c:axId val="1537403936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1314,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448487744"/>
+        <c:crossAx val="1537406496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1323,7 +1322,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448487744"/>
+        <c:axId val="1537406496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1373,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448253408"/>
+        <c:crossAx val="1537403936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1388,7 +1387,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1495,7 +1493,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1599,11 +1596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="751611488"/>
-        <c:axId val="496722240"/>
+        <c:axId val="1537520928"/>
+        <c:axId val="1537523408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="751611488"/>
+        <c:axId val="1537520928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1642,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496722240"/>
+        <c:crossAx val="1537523408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1653,7 +1650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496722240"/>
+        <c:axId val="1537523408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,7 +1701,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751611488"/>
+        <c:crossAx val="1537520928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1793,7 +1790,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1882,11 +1878,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="497115104"/>
-        <c:axId val="748388624"/>
+        <c:axId val="1537546944"/>
+        <c:axId val="1537549696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497115104"/>
+        <c:axId val="1537546944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,7 +1924,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="748388624"/>
+        <c:crossAx val="1537549696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1936,7 +1932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="748388624"/>
+        <c:axId val="1537549696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1987,7 +1983,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497115104"/>
+        <c:crossAx val="1537546944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2076,7 +2072,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2168,11 +2163,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="497138528"/>
-        <c:axId val="670747584"/>
+        <c:axId val="1537568928"/>
+        <c:axId val="1537571680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497138528"/>
+        <c:axId val="1537568928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2214,7 +2209,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="670747584"/>
+        <c:crossAx val="1537571680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2222,7 +2217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="670747584"/>
+        <c:axId val="1537571680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,7 +2268,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497138528"/>
+        <c:crossAx val="1537568928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2362,7 +2357,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2457,11 +2451,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="497003456"/>
-        <c:axId val="497005776"/>
+        <c:axId val="1537591040"/>
+        <c:axId val="1537593792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497003456"/>
+        <c:axId val="1537591040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2503,7 +2497,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497005776"/>
+        <c:crossAx val="1537593792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2511,7 +2505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497005776"/>
+        <c:axId val="1537593792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2561,7 +2555,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497003456"/>
+        <c:crossAx val="1537591040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2738,11 +2732,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="448525456"/>
-        <c:axId val="448527776"/>
+        <c:axId val="1537018656"/>
+        <c:axId val="1537021408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448525456"/>
+        <c:axId val="1537018656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2784,7 +2778,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448527776"/>
+        <c:crossAx val="1537021408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2792,7 +2786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448527776"/>
+        <c:axId val="1537021408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2843,7 +2837,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448525456"/>
+        <c:crossAx val="1537018656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2932,7 +2926,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3027,11 +3020,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="448336992"/>
-        <c:axId val="448338768"/>
+        <c:axId val="1537598816"/>
+        <c:axId val="1537601568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448336992"/>
+        <c:axId val="1537598816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3073,7 +3066,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448338768"/>
+        <c:crossAx val="1537601568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3081,7 +3074,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448338768"/>
+        <c:axId val="1537601568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3132,7 +3125,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448336992"/>
+        <c:crossAx val="1537598816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3326,11 +3319,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496498816"/>
-        <c:axId val="496500864"/>
+        <c:axId val="1537624416"/>
+        <c:axId val="1537627168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496498816"/>
+        <c:axId val="1537624416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3365,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496500864"/>
+        <c:crossAx val="1537627168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3380,7 +3373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496500864"/>
+        <c:axId val="1537627168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3431,7 +3424,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496498816"/>
+        <c:crossAx val="1537624416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3589,13 +3582,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>13584.0</c:v>
+                  <c:v>9402.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9372.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13857.0</c:v>
+                  <c:v>9372.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>9769.0</c:v>
@@ -3604,19 +3597,19 @@
                   <c:v>9326.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13845.0</c:v>
+                  <c:v>9368.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13558.0</c:v>
+                  <c:v>9359.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13852.0</c:v>
+                  <c:v>9357.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13692.0</c:v>
+                  <c:v>9341.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13842.0</c:v>
+                  <c:v>9342.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9325.0</c:v>
@@ -3625,16 +3618,16 @@
                   <c:v>9354.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14252.0</c:v>
+                  <c:v>10243.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>9436.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13707.0</c:v>
+                  <c:v>9369.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13756.0</c:v>
+                  <c:v>9419.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>9344.0</c:v>
@@ -3643,13 +3636,13 @@
                   <c:v>9384.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13719.0</c:v>
+                  <c:v>9381.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13688.0</c:v>
+                  <c:v>9344.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13557.0</c:v>
+                  <c:v>9357.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>9343.0</c:v>
@@ -3664,22 +3657,22 @@
                   <c:v>9349.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13585.0</c:v>
+                  <c:v>10268.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>9368.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13839.0</c:v>
+                  <c:v>9357.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13573.0</c:v>
+                  <c:v>10240.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>9373.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13714.0</c:v>
+                  <c:v>9380.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3825,11 +3818,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496089424"/>
-        <c:axId val="496091744"/>
+        <c:axId val="1537661744"/>
+        <c:axId val="1537664496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496089424"/>
+        <c:axId val="1537661744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3871,7 +3864,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496091744"/>
+        <c:crossAx val="1537664496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3879,7 +3872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496091744"/>
+        <c:axId val="1537664496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3985,7 +3978,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496089424"/>
+        <c:crossAx val="1537661744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4257,11 +4250,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="494929120"/>
-        <c:axId val="494931168"/>
+        <c:axId val="1537696032"/>
+        <c:axId val="1537698784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="494929120"/>
+        <c:axId val="1537696032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,7 +4296,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494931168"/>
+        <c:crossAx val="1537698784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4311,7 +4304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494931168"/>
+        <c:axId val="1537698784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4362,7 +4355,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494929120"/>
+        <c:crossAx val="1537696032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4626,11 +4619,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="749379376"/>
-        <c:axId val="749381696"/>
+        <c:axId val="1537724336"/>
+        <c:axId val="1537727088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="749379376"/>
+        <c:axId val="1537724336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4672,7 +4665,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749381696"/>
+        <c:crossAx val="1537727088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4680,7 +4673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="749381696"/>
+        <c:axId val="1537727088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4730,7 +4723,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749379376"/>
+        <c:crossAx val="1537724336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4825,7 +4818,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5364,11 +5356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="448410528"/>
-        <c:axId val="448412672"/>
+        <c:axId val="1536919344"/>
+        <c:axId val="1536922336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="448410528"/>
+        <c:axId val="1536919344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5410,7 +5402,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448412672"/>
+        <c:crossAx val="1536922336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5418,7 +5410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448412672"/>
+        <c:axId val="1536922336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5439,7 +5431,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5500,7 +5491,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448410528"/>
+        <c:crossAx val="1536919344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5807,13 +5798,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="1">
-                  <c:v>13584.0</c:v>
+                  <c:v>9402.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9372.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13857.0</c:v>
+                  <c:v>9372.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>9769.0</c:v>
@@ -5822,19 +5813,19 @@
                   <c:v>9326.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13845.0</c:v>
+                  <c:v>9368.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13558.0</c:v>
+                  <c:v>9359.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13852.0</c:v>
+                  <c:v>9357.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13692.0</c:v>
+                  <c:v>9341.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13842.0</c:v>
+                  <c:v>9342.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>9325.0</c:v>
@@ -5843,16 +5834,16 @@
                   <c:v>9354.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14252.0</c:v>
+                  <c:v>10243.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>9436.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13707.0</c:v>
+                  <c:v>9369.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13756.0</c:v>
+                  <c:v>9419.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>9344.0</c:v>
@@ -5861,13 +5852,13 @@
                   <c:v>9384.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13719.0</c:v>
+                  <c:v>9381.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13688.0</c:v>
+                  <c:v>9344.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13557.0</c:v>
+                  <c:v>9357.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>9343.0</c:v>
@@ -5882,22 +5873,22 @@
                   <c:v>9349.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13585.0</c:v>
+                  <c:v>10268.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>9368.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13839.0</c:v>
+                  <c:v>9357.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13573.0</c:v>
+                  <c:v>10240.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>9373.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13714.0</c:v>
+                  <c:v>9380.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5913,11 +5904,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="705572816"/>
-        <c:axId val="705574864"/>
+        <c:axId val="1537752832"/>
+        <c:axId val="1537755584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="705572816"/>
+        <c:axId val="1537752832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5959,7 +5950,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705574864"/>
+        <c:crossAx val="1537755584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5967,7 +5958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="705574864"/>
+        <c:axId val="1537755584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6073,7 +6064,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705572816"/>
+        <c:crossAx val="1537752832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6201,7 +6192,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6761,11 +6751,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="773672384"/>
-        <c:axId val="773602464"/>
+        <c:axId val="1536965248"/>
+        <c:axId val="1536968240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="773672384"/>
+        <c:axId val="1536965248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6807,7 +6797,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773602464"/>
+        <c:crossAx val="1536968240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6815,7 +6805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="773602464"/>
+        <c:axId val="1536968240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6836,7 +6826,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6897,7 +6886,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773672384"/>
+        <c:crossAx val="1536965248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7025,7 +7014,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7260,11 +7248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="773736560"/>
-        <c:axId val="773738880"/>
+        <c:axId val="1537001424"/>
+        <c:axId val="1537004176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="773736560"/>
+        <c:axId val="1537001424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7306,7 +7294,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773738880"/>
+        <c:crossAx val="1537004176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7314,7 +7302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="773738880"/>
+        <c:axId val="1537004176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7365,7 +7353,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7425,7 +7412,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773736560"/>
+        <c:crossAx val="1537001424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7654,11 +7641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="496316816"/>
-        <c:axId val="496348768"/>
+        <c:axId val="1537452784"/>
+        <c:axId val="1537455264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496316816"/>
+        <c:axId val="1537452784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7700,7 +7687,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496348768"/>
+        <c:crossAx val="1537455264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7708,7 +7695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496348768"/>
+        <c:axId val="1537455264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7759,7 +7746,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496316816"/>
+        <c:crossAx val="1537452784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7848,7 +7835,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7940,11 +7926,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496940592"/>
-        <c:axId val="496949904"/>
+        <c:axId val="1537475568"/>
+        <c:axId val="1537478320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496940592"/>
+        <c:axId val="1537475568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7986,7 +7972,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496949904"/>
+        <c:crossAx val="1537478320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7994,7 +7980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496949904"/>
+        <c:axId val="1537478320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8045,7 +8031,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496940592"/>
+        <c:crossAx val="1537475568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8134,7 +8120,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8229,11 +8214,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="496568336"/>
-        <c:axId val="496570656"/>
+        <c:axId val="1537503456"/>
+        <c:axId val="1537506208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="496568336"/>
+        <c:axId val="1537503456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8275,7 +8260,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496570656"/>
+        <c:crossAx val="1537506208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8283,7 +8268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496570656"/>
+        <c:axId val="1537506208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8333,7 +8318,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496568336"/>
+        <c:crossAx val="1537503456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8513,11 +8498,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="773065456"/>
-        <c:axId val="773067504"/>
+        <c:axId val="1467420752"/>
+        <c:axId val="1467387760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="773065456"/>
+        <c:axId val="1467420752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8559,7 +8544,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773067504"/>
+        <c:crossAx val="1467387760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8567,7 +8552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="773067504"/>
+        <c:axId val="1467387760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8617,7 +8602,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="773065456"/>
+        <c:crossAx val="1467420752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8706,7 +8691,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8801,11 +8785,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="497099648"/>
-        <c:axId val="497101968"/>
+        <c:axId val="1467766352"/>
+        <c:axId val="1467768400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="497099648"/>
+        <c:axId val="1467766352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8847,7 +8831,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497101968"/>
+        <c:crossAx val="1467768400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8855,7 +8839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497101968"/>
+        <c:axId val="1467768400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8905,7 +8889,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497099648"/>
+        <c:crossAx val="1467766352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27626,8 +27610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="84" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27712,7 +27696,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>4182</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -27725,7 +27709,7 @@
       </c>
       <c r="N3" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13584</v>
+        <v>9402</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -27802,7 +27786,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>8765</v>
+        <v>4280</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -27815,7 +27799,7 @@
       </c>
       <c r="N5" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13857</v>
+        <v>9372</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -27934,7 +27918,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>4477</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -27950,7 +27934,7 @@
       </c>
       <c r="N8" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13845</v>
+        <v>9368</v>
       </c>
       <c r="P8" t="s">
         <v>124</v>
@@ -27982,7 +27966,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>4199</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -27998,7 +27982,7 @@
       </c>
       <c r="N9" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13558</v>
+        <v>9359</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -28024,7 +28008,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>8760</v>
+        <v>4265</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -28043,7 +28027,7 @@
       </c>
       <c r="N10" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13852</v>
+        <v>9357</v>
       </c>
       <c r="P10" s="32"/>
       <c r="Q10" s="32" t="s">
@@ -28076,7 +28060,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>8612</v>
+        <v>4261</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -28095,7 +28079,7 @@
       </c>
       <c r="N11" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13692</v>
+        <v>9341</v>
       </c>
       <c r="P11" s="30" t="s">
         <v>75</v>
@@ -28130,7 +28114,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>8779</v>
+        <v>4279</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -28149,7 +28133,7 @@
       </c>
       <c r="N12" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13842</v>
+        <v>9342</v>
       </c>
       <c r="P12" s="30" t="s">
         <v>127</v>
@@ -28293,7 +28277,7 @@
         <v>5156</v>
       </c>
       <c r="I15">
-        <v>4009</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -28309,7 +28293,7 @@
       </c>
       <c r="N15" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>14252</v>
+        <v>10243</v>
       </c>
       <c r="P15" s="30" t="s">
         <v>130</v>
@@ -28397,10 +28381,10 @@
         <v>4272</v>
       </c>
       <c r="I17">
-        <v>875</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>3463</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -28413,7 +28397,7 @@
       </c>
       <c r="N17" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13707</v>
+        <v>9369</v>
       </c>
       <c r="P17" s="30" t="s">
         <v>132</v>
@@ -28449,7 +28433,7 @@
         <v>4248</v>
       </c>
       <c r="I18">
-        <v>4337</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -28465,7 +28449,7 @@
       </c>
       <c r="N18" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13756</v>
+        <v>9419</v>
       </c>
       <c r="P18" s="30" t="s">
         <v>133</v>
@@ -28602,10 +28586,10 @@
         <v>4281</v>
       </c>
       <c r="H21">
-        <v>875</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>3463</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <f>Puppet!K43</f>
@@ -28625,7 +28609,7 @@
       </c>
       <c r="N21" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13719</v>
+        <v>9381</v>
       </c>
       <c r="P21" s="33"/>
       <c r="Q21" s="33"/>
@@ -28657,7 +28641,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>4344</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -28673,7 +28657,7 @@
       </c>
       <c r="N22" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13688</v>
+        <v>9344</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
@@ -28699,10 +28683,10 @@
         <v>4247</v>
       </c>
       <c r="H23">
-        <v>875</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>3325</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -28718,7 +28702,7 @@
       </c>
       <c r="N23" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13557</v>
+        <v>9357</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -28927,7 +28911,7 @@
         <v>5163</v>
       </c>
       <c r="I28">
-        <v>3317</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -28943,7 +28927,7 @@
       </c>
       <c r="N28" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13585</v>
+        <v>10268</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -29014,7 +28998,7 @@
         <v>4268</v>
       </c>
       <c r="H30">
-        <v>4482</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -29033,7 +29017,7 @@
       </c>
       <c r="N30" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13839</v>
+        <v>9357</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
@@ -29062,7 +29046,7 @@
         <v>5134</v>
       </c>
       <c r="I31">
-        <v>3333</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -29078,7 +29062,7 @@
       </c>
       <c r="N31" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13573</v>
+        <v>10240</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -29149,7 +29133,7 @@
         <v>4285</v>
       </c>
       <c r="H33">
-        <v>4334</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -29168,11 +29152,11 @@
       </c>
       <c r="N33" s="19">
         <f>SUM(Tabel2[[#This Row],[T1]:[T13]])</f>
-        <v>13714</v>
+        <v>9380</v>
       </c>
       <c r="O33">
         <f>AVERAGE(N3,N5,N8:N12,N15,N17:N18,N21:N23,N28,N30,N31,N33)</f>
-        <v>13742.35294117647</v>
+        <v>9523.4705882352937</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -29181,7 +29165,7 @@
       </c>
       <c r="N34" s="5">
         <f>AVERAGE(N3:N33)</f>
-        <v>11777.903225806451</v>
+        <v>9464.322580645161</v>
       </c>
       <c r="O34">
         <f>AVERAGE(N4,N6:N7,N13:N14,N16,N19:N20,N24:N27,N29,N32)</f>

</xml_diff>